<commit_message>
FGSalesReport and RM BegBalance Report
Modified SP for FG and Sales Report
Added script for the SP and table of RM Beginning Balance Report
LSPDirectMaterial = added "Family" field in Finished Goods Report
LSP Direct Material Controller = change grouping of family, correction of formula in SalesSummary, change order by of grouping by Family and Product Code
</commit_message>
<xml_diff>
--- a/ERPReports/ERPReports/Areas/Reports/Templates/LSP_Rpt_DM_FinishedGoodsSalesReport.xlsx
+++ b/ERPReports/ERPReports/Areas/Reports/Templates/LSP_Rpt_DM_FinishedGoodsSalesReport.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8479E545-AC94-4631-A3CA-13A6607AED54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-2700" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINISHED GOODS" sheetId="1" r:id="rId1"/>
@@ -198,7 +199,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-10409]mm/dd/yyyy"/>
@@ -719,6 +720,79 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -740,58 +814,6 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -805,18 +827,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -829,29 +839,20 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1161,17 +1162,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E10" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
@@ -1196,99 +1197,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
     </row>
     <row r="2" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
     </row>
     <row r="3" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="49" t="s">
+      <c r="A3" s="67"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="49" t="s">
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="49" t="s">
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="70"/>
+      <c r="Y3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="50"/>
-      <c r="AA3" s="51"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="70"/>
     </row>
     <row r="4" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1848,18 +1849,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A2:AA2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="Q3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A6:AA6"/>
     <mergeCell ref="A7:AA7"/>
     <mergeCell ref="A9:AA9"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A1:AA1"/>
-    <mergeCell ref="A2:AA2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="Q3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.65000000000000013" bottom="0.23" header="0.65000000000000013" footer="0.23"/>
@@ -1871,7 +1872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
@@ -1900,109 +1901,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="47"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
       <c r="AD2" s="24"/>
       <c r="AE2" s="24"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="49" t="s">
+      <c r="A3" s="71"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="49" t="s">
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="50"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="49" t="s">
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="69"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="50"/>
-      <c r="AC3" s="51"/>
+      <c r="AB3" s="69"/>
+      <c r="AC3" s="70"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
     </row>
@@ -2506,7 +2507,7 @@
       <c r="AE16" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:AC6"/>
+  <autoFilter ref="A4:AC6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="6">
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="A2:AC2"/>
@@ -2525,11 +2526,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2543,41 +2544,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="77"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="75"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -2611,41 +2612,41 @@
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
-      <c r="D9" s="78" t="s">
+      <c r="D9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
-      <c r="D10" s="78" t="s">
+      <c r="D10" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>